<commit_message>
add examples to template
</commit_message>
<xml_diff>
--- a/templates/community/CEPLAS-data/Golden_Gate_cloning.xlsx
+++ b/templates/community/CEPLAS-data/Golden_Gate_cloning.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="isa_template" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="New Table" state="visible" r:id="rId5"/>
+    <sheet sheetId="2" name="Golden_gate_cloning" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="80">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Golden_Gate_cloning</t>
+    <t>Golden Gate cloning</t>
   </si>
   <si>
     <t>Version</t>
@@ -38,7 +38,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>A template to describe Golden Gate cloning according to protocols from AG Eva Nowack.</t>
+    <t>A template to describe preparation of Golden Gate cloning mix according to protocols from AG Eva Nowack.</t>
   </si>
   <si>
     <t>Organisation</t>
@@ -50,7 +50,7 @@
     <t>Table</t>
   </si>
   <si>
-    <t>New Table</t>
+    <t>Golden_gate_cloning</t>
   </si>
   <si>
     <t>ERS</t>
@@ -197,16 +197,61 @@
     <t/>
   </si>
   <si>
-    <t>Femtomole</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C68854</t>
+    <t>T4 Ligase Buffer</t>
+  </si>
+  <si>
+    <t>10x</t>
+  </si>
+  <si>
+    <t>1.5</t>
   </si>
   <si>
     <t>Microliter</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C48153</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>cloning_master_mix</t>
+  </si>
+  <si>
+    <t>T4 Ligase</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>BsaI-HFv2</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>destination plasmid</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>femtomolar</t>
+  </si>
+  <si>
+    <t>UO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000073</t>
+  </si>
+  <si>
+    <t>to be calculated</t>
+  </si>
+  <si>
+    <t>insert(s)</t>
+  </si>
+  <si>
+    <t>ddH2O</t>
   </si>
 </sst>
 </file>
@@ -262,8 +307,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:U2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:U2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:U7" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:U7">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -792,7 +837,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -868,7 +913,7 @@
         <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>60</v>
@@ -877,7 +922,7 @@
         <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
         <v>60</v>
@@ -889,40 +934,365 @@
         <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O2" t="s">
         <v>23</v>
       </c>
       <c r="P2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" t="s">
         <v>64</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>60</v>
-      </c>
-      <c r="R2" t="s">
-        <v>63</v>
       </c>
       <c r="S2" t="s">
         <v>23</v>
       </c>
       <c r="T2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" t="s">
         <v>64</v>
       </c>
-      <c r="U2" t="s">
-        <v>60</v>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" t="s">
+        <v>65</v>
+      </c>
+      <c r="U3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" t="s">
+        <v>64</v>
+      </c>
+      <c r="S4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" t="s">
+        <v>64</v>
+      </c>
+      <c r="S5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>66</v>
+      </c>
+      <c r="R6" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" t="s">
+        <v>64</v>
+      </c>
+      <c r="S7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>